<commit_message>
export separate ro and  roo
</commit_message>
<xml_diff>
--- a/ro_export_date.xlsx
+++ b/ro_export_date.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -52,10 +52,10 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Regional Order</t>
+    <t>Regional Office Order</t>
   </si>
   <si>
-    <t>2020-006</t>
+    <t>2020-005</t>
   </si>
   <si>
     <t>July 21, 2020</t>
@@ -68,18 +68,6 @@
   </si>
   <si>
     <t>cvferrer</t>
-  </si>
-  <si>
-    <t>Regional Office Order</t>
-  </si>
-  <si>
-    <t>2020-005</t>
-  </si>
-  <si>
-    <t>2020-007</t>
-  </si>
-  <si>
-    <t>cancelled</t>
   </si>
 </sst>
 </file>
@@ -713,78 +701,34 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:9" customHeight="1" ht="37.5">
-      <c r="A9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:9" customHeight="1" ht="37.5">
-      <c r="A10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:9" customHeight="1" ht="37.5">
-      <c r="A11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>20</v>
-      </c>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:9" customHeight="1" ht="37.5">
       <c r="A12" s="16"/>

</xml_diff>